<commit_message>
Se acomodo el codigo y se completo la matriz con AS faltantes.
</commit_message>
<xml_diff>
--- a/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
+++ b/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauro\Desktop\Compiladores\Entrega 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpaces\REPO-Compiladores\Cursada\Entregas\Entrega n°1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11895" windowHeight="5880"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -122,9 +122,6 @@
     <t>}</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>"</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>AS-13</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H3" workbookViewId="0">
-      <selection activeCell="V22" sqref="T22:V22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,19 +905,19 @@
         <v>31</v>
       </c>
       <c r="R2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="S2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="T2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="17" t="s">
-        <v>34</v>
-      </c>
       <c r="U2" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
@@ -931,16 +931,16 @@
         <v>10</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>1</v>
@@ -952,28 +952,28 @@
         <v>3</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>6</v>
@@ -985,36 +985,36 @@
         <v>0</v>
       </c>
       <c r="V3" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35"/>
       <c r="B4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="J4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -1022,7 +1022,7 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T4" s="6"/>
       <c r="U4" s="22"/>
@@ -1033,67 +1033,67 @@
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U5" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V5" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1125,67 +1125,67 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U7" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V7" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1217,67 +1217,67 @@
         <v>3</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U9" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V9" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1309,67 +1309,67 @@
         <v>4</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U11" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V11" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1545,10 +1545,10 @@
         <v>6</v>
       </c>
       <c r="S15" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T15" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U15" s="21" t="s">
         <v>6</v>
@@ -1560,65 +1560,65 @@
     <row r="16" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T16" s="6"/>
       <c r="U16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -1677,10 +1677,10 @@
         <v>6</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T17" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U17" s="25" t="s">
         <v>6</v>
@@ -1692,65 +1692,65 @@
     <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -1809,7 +1809,7 @@
         <v>6</v>
       </c>
       <c r="S19" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T19" s="3" t="s">
         <v>6</v>
@@ -1824,67 +1824,67 @@
     <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -1943,7 +1943,7 @@
         <v>6</v>
       </c>
       <c r="S21" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T21" s="13" t="s">
         <v>6</v>
@@ -1958,67 +1958,67 @@
     <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="33"/>
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T22" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="U22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -2026,133 +2026,133 @@
         <v>10</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U23" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V23" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="35"/>
       <c r="B24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -2160,133 +2160,133 @@
         <v>11</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R25" s="13" t="s">
         <v>12</v>
       </c>
       <c r="S25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U25" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V25" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="33"/>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -2294,7 +2294,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>14</v>
@@ -2306,68 +2306,68 @@
         <v>13</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U27" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V27" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35"/>
       <c r="B28" s="6"/>
       <c r="C28" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
@@ -2392,74 +2392,74 @@
         <v>13</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U29" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V29" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="33"/>
       <c r="B30" s="10"/>
       <c r="C30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -2486,133 +2486,133 @@
         <v>14</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U31" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V31" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35"/>
       <c r="B32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
@@ -2626,58 +2626,58 @@
         <v>15</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N33" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T33" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U33" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V33" s="29" t="s">
         <v>15</v>
@@ -2686,67 +2686,67 @@
     <row r="34" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="33"/>
       <c r="B34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V34" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Se realizaron correcciones sobre las AS
</commit_message>
<xml_diff>
--- a/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
+++ b/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="53">
   <si>
     <t>E00</t>
   </si>
@@ -176,10 +176,13 @@
     <t>AS-12</t>
   </si>
   <si>
-    <t>AS-13</t>
-  </si>
-  <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>AS-FINAL</t>
+  </si>
+  <si>
+    <t>AS-ERROR</t>
   </si>
 </sst>
 </file>
@@ -474,9 +477,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -547,20 +547,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -844,84 +847,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="22" max="22" width="11.42578125" style="28"/>
+    <col min="22" max="22" width="11.42578125" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="S2" s="16" t="s">
+      <c r="R2" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="T2" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="20" t="s">
+      <c r="U2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="V2" s="18" t="s">
+      <c r="V2" s="17" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -930,16 +933,16 @@
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -951,28 +954,28 @@
       <c r="J3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="8" t="s">
+      <c r="K3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>34</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" s="19" t="s">
+      <c r="N3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="18" t="s">
         <v>36</v>
       </c>
       <c r="S3" s="3" t="s">
@@ -981,27 +984,33 @@
       <c r="T3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="U3" s="21" t="s">
+      <c r="U3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="V3" s="30" t="s">
+      <c r="V3" s="29" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="D4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="F4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="H4" s="5" t="s">
         <v>43</v>
       </c>
@@ -1011,486 +1020,670 @@
       <c r="J4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
+      <c r="K4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="M4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
+      <c r="N4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="S4" s="5" t="s">
         <v>46</v>
       </c>
       <c r="T4" s="6"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="7"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="V5" s="9" t="s">
+      <c r="B5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="V5" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="11"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="U7" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="V7" s="9" t="s">
+      <c r="B7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="22"/>
-      <c r="V8" s="7"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="S9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="U9" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="V9" s="9" t="s">
+      <c r="B9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U9" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="V9" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="33"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="11"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="8" t="s">
+      <c r="B11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="S11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="U11" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="V11" s="9" t="s">
+      <c r="G11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="V11" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="7"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="12" t="s">
+      <c r="M13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="N13" s="12" t="s">
+      <c r="N13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O13" s="12" t="s">
+      <c r="O13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="P13" s="12" t="s">
+      <c r="P13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Q13" s="12" t="s">
+      <c r="Q13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="R13" s="12" t="s">
+      <c r="R13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="S13" s="12" t="s">
+      <c r="S13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="T13" s="13" t="s">
+      <c r="T13" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="U13" s="25" t="s">
+      <c r="U13" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="V13" s="14" t="s">
+      <c r="V13" s="13" t="s">
         <v>5</v>
       </c>
       <c r="XFD13" s="2"/>
     </row>
     <row r="14" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="33"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="11"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="10"/>
     </row>
     <row r="15" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1544,13 +1737,13 @@
       <c r="R15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U15" s="21" t="s">
+      <c r="S15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T15" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="U15" s="20" t="s">
         <v>6</v>
       </c>
       <c r="V15" s="4" t="s">
@@ -1558,7 +1751,7 @@
       </c>
     </row>
     <row r="16" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="5" t="s">
         <v>47</v>
       </c>
@@ -1611,9 +1804,11 @@
         <v>47</v>
       </c>
       <c r="S16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="T16" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="U16" s="5" t="s">
         <v>47</v>
       </c>
@@ -1622,75 +1817,75 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="M17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="N17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="O17" s="13" t="s">
+      <c r="B17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="P17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="R17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="S17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U17" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="V17" s="14" t="s">
+      <c r="P17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T17" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="U17" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="V17" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="33"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
@@ -1742,10 +1937,12 @@
       <c r="R18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="S18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T18" s="10"/>
+      <c r="S18" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="T18" s="36" t="s">
+        <v>52</v>
+      </c>
       <c r="U18" s="1" t="s">
         <v>47</v>
       </c>
@@ -1754,7 +1951,7 @@
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1808,13 +2005,13 @@
       <c r="R19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S19" s="8" t="s">
+      <c r="S19" s="7" t="s">
         <v>34</v>
       </c>
       <c r="T19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="U19" s="21" t="s">
+      <c r="U19" s="20" t="s">
         <v>6</v>
       </c>
       <c r="V19" s="4" t="s">
@@ -1822,7 +2019,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="5" t="s">
         <v>47</v>
       </c>
@@ -1875,222 +2072,222 @@
         <v>47</v>
       </c>
       <c r="S20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="U20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V20" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="P21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="U21" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="V21" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="32"/>
+      <c r="B22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="U20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="V20" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="L21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="M21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="N21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="O21" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="P21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="R21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="S21" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="U21" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="V21" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="33"/>
-      <c r="B22" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>47</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="S22" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="S22" s="36" t="s">
+        <v>51</v>
+      </c>
       <c r="T22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L23" s="8" t="s">
+      <c r="D23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23" s="7" t="s">
         <v>34</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="O23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="S23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="U23" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="V23" s="9" t="s">
+      <c r="N23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="V23" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="5" t="s">
         <v>48</v>
       </c>
@@ -2156,75 +2353,75 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="13" t="s">
+      <c r="B25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="O25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R25" s="13" t="s">
+      <c r="D25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R25" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="S25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="U25" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="V25" s="9" t="s">
+      <c r="S25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U25" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="V25" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="33"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="1" t="s">
         <v>48</v>
       </c>
@@ -2290,10 +2487,10 @@
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2305,61 +2502,63 @@
       <c r="E27" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="J27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="T27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U27" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="V27" s="30" t="s">
+      <c r="F27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="M27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="N27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="O27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="P27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="R27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="S27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="T27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="U27" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="V27" s="29" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="C28" s="5" t="s">
         <v>42</v>
       </c>
@@ -2369,188 +2568,262 @@
       <c r="E28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6"/>
-      <c r="U28" s="22"/>
-      <c r="V28" s="7"/>
+      <c r="F28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="S28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="T28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V28" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="J29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="T29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U29" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="V29" s="30" t="s">
+      <c r="D29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="L29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="M29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="N29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="O29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="P29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="R29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="S29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="T29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="U29" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="V29" s="29" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="33"/>
-      <c r="B30" s="10"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="36" t="s">
+        <v>52</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="11"/>
+      <c r="D30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="J30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="K30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="L30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="M30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="N30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="O30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="P30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="R30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="S30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="T30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="U30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="V30" s="36" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="O31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="S31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="U31" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="V31" s="9" t="s">
+      <c r="D31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U31" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="V31" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="5" t="s">
         <v>48</v>
       </c>
@@ -2616,75 +2889,75 @@
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J33" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="L33" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M33" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N33" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="O33" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="P33" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q33" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R33" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="S33" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T33" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="U33" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="V33" s="29" t="s">
+      <c r="D33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J33" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N33" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="O33" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="P33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T33" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="U33" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="V33" s="28" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="33"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="1" t="s">
         <v>39</v>
       </c>
@@ -2745,7 +3018,7 @@
       <c r="U34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V34" s="31" t="s">
+      <c r="V34" s="30" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2754,12 +3027,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A15:A16"/>
@@ -2770,6 +3037,12 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se probo y reviso el Lexico y funca.. falta ver AS's y los numeros..
</commit_message>
<xml_diff>
--- a/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
+++ b/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
@@ -155,34 +155,34 @@
     <t>AS-05</t>
   </si>
   <si>
+    <t>AS-07</t>
+  </si>
+  <si>
+    <t>AS-08</t>
+  </si>
+  <si>
+    <t>AS-09</t>
+  </si>
+  <si>
+    <t>AS-10</t>
+  </si>
+  <si>
+    <t>AS-11</t>
+  </si>
+  <si>
+    <t>AS-12</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>AS-FINAL</t>
+  </si>
+  <si>
+    <t>AS-ERROR</t>
+  </si>
+  <si>
     <t>AS-06</t>
-  </si>
-  <si>
-    <t>AS-07</t>
-  </si>
-  <si>
-    <t>AS-08</t>
-  </si>
-  <si>
-    <t>AS-09</t>
-  </si>
-  <si>
-    <t>AS-10</t>
-  </si>
-  <si>
-    <t>AS-11</t>
-  </si>
-  <si>
-    <t>AS-12</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>AS-FINAL</t>
-  </si>
-  <si>
-    <t>AS-ERROR</t>
   </si>
 </sst>
 </file>
@@ -547,6 +547,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -561,9 +564,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +908,7 @@
         <v>31</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S2" s="15" t="s">
         <v>32</v>
@@ -924,7 +924,7 @@
       </c>
     </row>
     <row r="3" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -992,7 +992,7 @@
       </c>
     </row>
     <row r="4" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="5" t="s">
         <v>38</v>
       </c>
@@ -1000,61 +1000,61 @@
         <v>41</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="J4" s="5" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T4" s="6"/>
       <c r="U4" s="21"/>
       <c r="V4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1122,73 +1122,73 @@
       </c>
     </row>
     <row r="6" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="34" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1256,73 +1256,73 @@
       </c>
     </row>
     <row r="8" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1390,73 +1390,73 @@
       </c>
     </row>
     <row r="10" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -1524,73 +1524,73 @@
       </c>
     </row>
     <row r="12" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -1659,7 +1659,7 @@
       <c r="XFD13" s="2"/>
     </row>
     <row r="14" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1683,7 +1683,7 @@
       <c r="V14" s="10"/>
     </row>
     <row r="15" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1751,73 +1751,73 @@
       </c>
     </row>
     <row r="16" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -1885,73 +1885,73 @@
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="S18" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="T18" s="36" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="S18" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="T18" s="31" t="s">
+        <v>51</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -2019,73 +2019,73 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -2153,73 +2153,73 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="S22" s="36" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="S22" s="31" t="s">
+        <v>50</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="34" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -2287,73 +2287,73 @@
       </c>
     </row>
     <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -2421,73 +2421,73 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="32"/>
+      <c r="A26" s="33"/>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="34" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="18" t="s">
@@ -2555,73 +2555,73 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="34"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="32" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="18" t="s">
@@ -2689,73 +2689,73 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="32"/>
-      <c r="B30" s="36" t="s">
-        <v>52</v>
+      <c r="A30" s="33"/>
+      <c r="B30" s="31" t="s">
+        <v>51</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="F30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="H30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="I30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="J30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="K30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="L30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="M30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="N30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="O30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="P30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="R30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="S30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="T30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="U30" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="V30" s="36" t="s">
-        <v>52</v>
+      <c r="D30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="K30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="L30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="M30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="N30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="P30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="R30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="S30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="T30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="U30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="V30" s="31" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -2823,73 +2823,73 @@
       </c>
     </row>
     <row r="32" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="34"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="36" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="26" t="s">
@@ -2957,7 +2957,7 @@
       </c>
     </row>
     <row r="34" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="32"/>
+      <c r="A34" s="33"/>
       <c r="B34" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Se acomodó la AS de lo LONG.
</commit_message>
<xml_diff>
--- a/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
+++ b/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="55">
   <si>
     <t>E00</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>AS-Descarta</t>
+  </si>
+  <si>
+    <t>AS-13</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -556,7 +559,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -842,7 +845,7 @@
   <dimension ref="A1:XFD35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A23" sqref="A23:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,7 +1051,7 @@
       </c>
     </row>
     <row r="5" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1316,7 +1319,7 @@
       </c>
     </row>
     <row r="9" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1584,7 +1587,7 @@
       </c>
     </row>
     <row r="13" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1853,7 +1856,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -2121,7 +2124,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -2325,71 +2328,71 @@
     <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="32"/>
       <c r="B24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>46</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="U24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="V24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -2657,7 +2660,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="16" t="s">
@@ -2925,7 +2928,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="23" t="s">
@@ -3063,12 +3066,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A15:A16"/>
@@ -3079,6 +3076,12 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregaron los Doubles..
</commit_message>
<xml_diff>
--- a/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
+++ b/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="56">
   <si>
     <t>E00</t>
   </si>
@@ -173,9 +173,6 @@
     <t>AS-12</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>AS-FINAL</t>
   </si>
   <si>
@@ -189,6 +186,12 @@
   </si>
   <si>
     <t>AS-13</t>
+  </si>
+  <si>
+    <t>AS-14</t>
+  </si>
+  <si>
+    <t>E, e</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -559,7 +562,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -844,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A24"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +908,7 @@
         <v>31</v>
       </c>
       <c r="R2" s="13" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="S2" s="13" t="s">
         <v>32</v>
@@ -997,49 +1000,49 @@
         <v>41</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>43</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>45</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>45</v>
@@ -1047,11 +1050,11 @@
       <c r="T4" s="6"/>
       <c r="U4" s="19"/>
       <c r="V4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="33" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1139,7 +1142,7 @@
         <v>47</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>47</v>
@@ -1273,13 +1276,13 @@
         <v>47</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>47</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>47</v>
@@ -1319,7 +1322,7 @@
       </c>
     </row>
     <row r="9" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1407,7 +1410,7 @@
         <v>47</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>47</v>
@@ -1587,7 +1590,7 @@
       </c>
     </row>
     <row r="13" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="33" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1658,67 +1661,67 @@
     <row r="14" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
@@ -1843,10 +1846,10 @@
         <v>46</v>
       </c>
       <c r="S16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U16" s="5" t="s">
         <v>46</v>
@@ -1856,7 +1859,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -1977,10 +1980,10 @@
         <v>46</v>
       </c>
       <c r="S18" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T18" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>46</v>
@@ -2111,7 +2114,7 @@
         <v>46</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T20" s="5" t="s">
         <v>46</v>
@@ -2124,7 +2127,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -2245,7 +2248,7 @@
         <v>48</v>
       </c>
       <c r="S22" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>48</v>
@@ -2328,71 +2331,71 @@
     <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="32"/>
       <c r="B24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>46</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="33" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -2462,67 +2465,67 @@
     <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30"/>
       <c r="B26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="R26" s="1" t="s">
         <v>46</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -2596,7 +2599,7 @@
     <row r="28" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="32"/>
       <c r="B28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>42</v>
@@ -2608,59 +2611,59 @@
         <v>46</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="16" t="s">
@@ -2730,67 +2733,67 @@
     <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="30"/>
       <c r="B30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V30" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
@@ -2928,7 +2931,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="23" t="s">
@@ -3066,6 +3069,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A15:A16"/>
@@ -3076,12 +3085,6 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Lexico corregido todo todito
</commit_message>
<xml_diff>
--- a/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
+++ b/Cursada/Entregas/Entrega n°1/TP1 - Matriz de transición de estados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpaces\REPO-Compiladores\Cursada\Entregas\Entrega n°1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\REPO-Git\Compiladores\Cursada\Entregas\Entrega n°1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="52">
   <si>
     <t>E00</t>
   </si>
@@ -167,12 +167,6 @@
     <t>AS-10</t>
   </si>
   <si>
-    <t>AS-11</t>
-  </si>
-  <si>
-    <t>AS-12</t>
-  </si>
-  <si>
     <t>AS-FINAL</t>
   </si>
   <si>
@@ -185,23 +179,14 @@
     <t>AS-Descarta</t>
   </si>
   <si>
-    <t>AS-13</t>
-  </si>
-  <si>
-    <t>AS-14</t>
-  </si>
-  <si>
     <t>E, e</t>
-  </si>
-  <si>
-    <t>AS-15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,15 +204,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -562,6 +538,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -576,9 +555,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +899,7 @@
         <v>31</v>
       </c>
       <c r="R2" s="13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="S2" s="13" t="s">
         <v>32</v>
@@ -939,7 +915,7 @@
       </c>
     </row>
     <row r="3" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1007,69 +983,69 @@
       </c>
     </row>
     <row r="4" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>43</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="T4" s="6"/>
       <c r="U4" s="19"/>
       <c r="V4" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1137,341 +1113,341 @@
       </c>
     </row>
     <row r="6" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="I6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="33"/>
+      <c r="B8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="I8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="K8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U9" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="31"/>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="S7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="U7" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="V7" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="R8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="V8" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="T9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="U9" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="V9" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
-      <c r="B10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="32" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -1539,73 +1515,73 @@
       </c>
     </row>
     <row r="12" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="30" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1674,73 +1650,73 @@
       <c r="XFD13" s="2"/>
     </row>
     <row r="14" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="32" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1808,73 +1784,73 @@
       </c>
     </row>
     <row r="16" spans="1:22 16384:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="S16" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -1942,73 +1918,73 @@
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="S18" s="28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T18" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -2076,73 +2052,73 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="30" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -2210,73 +2186,73 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="Q22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S22" s="28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="32" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -2344,73 +2320,73 @@
       </c>
     </row>
     <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="32"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="U24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="V24" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -2478,73 +2454,73 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="32" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -2612,73 +2588,73 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="32"/>
-      <c r="B28" s="5" t="s">
-        <v>56</v>
+      <c r="A28" s="33"/>
+      <c r="B28" s="29" t="s">
+        <v>39</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="I28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="K28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="L28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="M28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="N28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="O28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="P28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="R28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="S28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="T28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="U28" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="V28" s="34" t="s">
-        <v>56</v>
+        <v>38</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="M28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="N28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="O28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="P28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="R28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="S28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="T28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="U28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="V28" s="29" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="16" t="s">
@@ -2746,73 +2722,73 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="30"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="32" t="s">
         <v>14</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -2880,73 +2856,73 @@
       </c>
     </row>
     <row r="32" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="32"/>
+      <c r="A32" s="33"/>
       <c r="B32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="S32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="T32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="V32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="34" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="23" t="s">
@@ -3014,12 +2990,12 @@
       </c>
     </row>
     <row r="34" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="30"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -3076,7 +3052,7 @@
         <v>40</v>
       </c>
       <c r="V34" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>